<commit_message>
Uploaded new/fixed data from babylab_princeton and infantlanglab_utk, per #46
</commit_message>
<xml_diff>
--- a/processed_data/participants_cleaned/infantlanglab_utk_participant data_12 to 15 mnths_gaze following.xlsx
+++ b/processed_data/participants_cleaned/infantlanglab_utk_participant data_12 to 15 mnths_gaze following.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InfantLanguageLab\Documents\ILPLL\LabProjects\EyeGaze\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InfantLanguageLab\Documents\ILPLL\LabProjects\EyeGaze\UploadedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9023CBC-3A8D-4F6D-A7A1-234F6826B293}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="12-15 mos" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -202,9 +201,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>Preterm</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -296,12 +292,15 @@
   </si>
   <si>
     <t>Matlab was jittery.</t>
+  </si>
+  <si>
+    <t>error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -668,11 +667,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -685,7 +684,8 @@
     <col min="8" max="8" width="24.25" customWidth="1"/>
     <col min="9" max="9" width="16.125" style="6" customWidth="1"/>
     <col min="10" max="10" width="13.875" customWidth="1"/>
-    <col min="11" max="19" width="8.5" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="19" width="8.5" customWidth="1"/>
     <col min="20" max="20" width="11.25" customWidth="1"/>
     <col min="21" max="21" width="8.625" customWidth="1"/>
     <col min="22" max="22" width="11.25" customWidth="1"/>
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -728,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -877,7 +877,7 @@
         <v>52</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>53</v>
@@ -934,7 +934,7 @@
         <v>16</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AC2" s="3">
         <v>5</v>
@@ -943,16 +943,16 @@
         <v>0</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>53</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>53</v>
@@ -1005,7 +1005,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>49</v>
@@ -1026,7 +1026,7 @@
         <v>52</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>53</v>
@@ -1082,8 +1082,8 @@
       <c r="AA3" s="3">
         <v>18</v>
       </c>
-      <c r="AB3" s="2" t="s">
-        <v>64</v>
+      <c r="AB3" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>53</v>
@@ -1092,16 +1092,16 @@
         <v>1</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI3" s="3" t="s">
         <v>53</v>
@@ -1154,7 +1154,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>49</v>
@@ -1175,7 +1175,7 @@
         <v>52</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>53</v>
@@ -1232,7 +1232,7 @@
         <v>16</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AC4" s="3">
         <v>6</v>
@@ -1241,16 +1241,16 @@
         <v>0</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG4" s="3" t="s">
         <v>53</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI4" s="3" t="s">
         <v>53</v>
@@ -1303,13 +1303,13 @@
         <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="3">
         <v>399</v>
@@ -1324,7 +1324,7 @@
         <v>52</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>53</v>
@@ -1381,7 +1381,7 @@
         <v>18</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC5" s="3" t="s">
         <v>53</v>
@@ -1390,16 +1390,16 @@
         <v>0</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG5" s="3" t="s">
         <v>53</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI5" s="3" t="s">
         <v>53</v>
@@ -1452,13 +1452,13 @@
         <v>44</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="5">
         <v>369</v>
@@ -1473,7 +1473,7 @@
         <v>52</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>53</v>
@@ -1488,7 +1488,7 @@
         <v>100</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>53</v>
@@ -1515,7 +1515,7 @@
         <v>57</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>57</v>
@@ -1529,8 +1529,8 @@
       <c r="AA6" s="5">
         <v>13</v>
       </c>
-      <c r="AB6" s="5" t="s">
-        <v>60</v>
+      <c r="AB6" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC6" s="5">
         <v>10</v>
@@ -1539,16 +1539,16 @@
         <v>0</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG6" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI6" s="5" t="s">
         <v>53</v>
@@ -1601,7 +1601,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>49</v>
@@ -1622,7 +1622,7 @@
         <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>53</v>
@@ -1678,8 +1678,8 @@
       <c r="AA7" s="5">
         <v>12</v>
       </c>
-      <c r="AB7" s="5" t="s">
-        <v>60</v>
+      <c r="AB7" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC7" s="5">
         <v>12</v>
@@ -1688,16 +1688,16 @@
         <v>5</v>
       </c>
       <c r="AE7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG7" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI7" s="5" t="s">
         <v>53</v>
@@ -1750,7 +1750,7 @@
         <v>44</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>49</v>
@@ -1768,10 +1768,10 @@
         <v>51</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>53</v>
@@ -1827,8 +1827,8 @@
       <c r="AA8" s="5">
         <v>16</v>
       </c>
-      <c r="AB8" s="7" t="s">
-        <v>64</v>
+      <c r="AB8" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC8" s="7" t="s">
         <v>53</v>
@@ -1837,16 +1837,16 @@
         <v>0</v>
       </c>
       <c r="AE8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG8" s="7" t="s">
         <v>53</v>
       </c>
       <c r="AH8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI8" s="7" t="s">
         <v>53</v>
@@ -1899,13 +1899,13 @@
         <v>44</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="5">
         <v>387</v>
@@ -1917,10 +1917,10 @@
         <v>51</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>53</v>
@@ -1976,8 +1976,8 @@
       <c r="AA9" s="5">
         <v>21</v>
       </c>
-      <c r="AB9" s="7" t="s">
-        <v>64</v>
+      <c r="AB9" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC9" s="7" t="s">
         <v>53</v>
@@ -1986,16 +1986,16 @@
         <v>0</v>
       </c>
       <c r="AE9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG9" s="7" t="s">
         <v>53</v>
       </c>
       <c r="AH9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI9" s="7" t="s">
         <v>53</v>
@@ -2048,13 +2048,13 @@
         <v>44</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="5">
         <v>428</v>
@@ -2069,7 +2069,7 @@
         <v>52</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>53</v>
@@ -2125,8 +2125,8 @@
       <c r="AA10" s="5">
         <v>13</v>
       </c>
-      <c r="AB10" s="5" t="s">
-        <v>60</v>
+      <c r="AB10" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC10" s="5">
         <v>12</v>
@@ -2135,19 +2135,19 @@
         <v>0</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG10" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI10" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="AI10" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="AJ10" s="5">
         <v>5</v>
@@ -2197,13 +2197,13 @@
         <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="5">
         <v>424</v>
@@ -2218,7 +2218,7 @@
         <v>52</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>53</v>
@@ -2260,7 +2260,7 @@
         <v>59</v>
       </c>
       <c r="W11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X11" s="5" t="s">
         <v>59</v>
@@ -2274,8 +2274,8 @@
       <c r="AA11" s="5">
         <v>20</v>
       </c>
-      <c r="AB11" s="5" t="s">
-        <v>60</v>
+      <c r="AB11" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC11" s="5">
         <v>3</v>
@@ -2284,16 +2284,16 @@
         <v>2</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF11" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG11" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH11" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI11" s="5" t="s">
         <v>53</v>
@@ -2346,13 +2346,13 @@
         <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="5">
         <v>439</v>
@@ -2367,7 +2367,7 @@
         <v>52</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>53</v>
@@ -2423,8 +2423,8 @@
       <c r="AA12" s="5">
         <v>16</v>
       </c>
-      <c r="AB12" s="5" t="s">
-        <v>60</v>
+      <c r="AB12" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC12" s="5">
         <v>7</v>
@@ -2433,16 +2433,16 @@
         <v>2</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG12" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI12" s="5" t="s">
         <v>53</v>
@@ -2495,13 +2495,13 @@
         <v>44</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="5">
         <v>435</v>
@@ -2516,7 +2516,7 @@
         <v>52</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>53</v>
@@ -2558,7 +2558,7 @@
         <v>59</v>
       </c>
       <c r="W13" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X13" s="5" t="s">
         <v>57</v>
@@ -2572,8 +2572,8 @@
       <c r="AA13" s="5">
         <v>18</v>
       </c>
-      <c r="AB13" s="5" t="s">
-        <v>60</v>
+      <c r="AB13" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC13" s="5">
         <v>8</v>
@@ -2582,16 +2582,16 @@
         <v>0</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF13" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG13" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH13" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI13" s="5" t="s">
         <v>53</v>
@@ -2644,7 +2644,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>49</v>
@@ -2665,7 +2665,7 @@
         <v>52</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>53</v>
@@ -2721,8 +2721,8 @@
       <c r="AA14" s="5">
         <v>8</v>
       </c>
-      <c r="AB14" s="5" t="s">
-        <v>64</v>
+      <c r="AB14" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC14" s="5" t="s">
         <v>53</v>
@@ -2731,16 +2731,16 @@
         <v>0</v>
       </c>
       <c r="AE14" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF14" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG14" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH14" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI14" s="5" t="s">
         <v>53</v>
@@ -2793,7 +2793,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>49</v>
@@ -2814,7 +2814,7 @@
         <v>52</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>53</v>
@@ -2870,8 +2870,8 @@
       <c r="AA15" s="5">
         <v>12</v>
       </c>
-      <c r="AB15" s="5" t="s">
-        <v>60</v>
+      <c r="AB15" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC15" s="5">
         <v>3</v>
@@ -2880,16 +2880,16 @@
         <v>0</v>
       </c>
       <c r="AE15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG15" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI15" s="5" t="s">
         <v>53</v>
@@ -2942,13 +2942,13 @@
         <v>44</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="5">
         <v>427</v>
@@ -2963,7 +2963,7 @@
         <v>52</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>53</v>
@@ -3019,8 +3019,8 @@
       <c r="AA16" s="5">
         <v>16</v>
       </c>
-      <c r="AB16" s="5" t="s">
-        <v>60</v>
+      <c r="AB16" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC16" s="5">
         <v>2</v>
@@ -3029,16 +3029,16 @@
         <v>0</v>
       </c>
       <c r="AE16" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF16" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG16" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH16" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI16" s="5" t="s">
         <v>53</v>
@@ -3091,13 +3091,13 @@
         <v>44</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="5">
         <v>415</v>
@@ -3106,13 +3106,13 @@
         <v>4</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>53</v>
@@ -3168,8 +3168,8 @@
       <c r="AA17" s="5">
         <v>18</v>
       </c>
-      <c r="AB17" s="5" t="s">
-        <v>60</v>
+      <c r="AB17" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC17" s="5">
         <v>7</v>
@@ -3178,16 +3178,16 @@
         <v>0</v>
       </c>
       <c r="AE17" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF17" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG17" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH17" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI17" s="5" t="s">
         <v>53</v>
@@ -3240,7 +3240,7 @@
         <v>44</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>49</v>
@@ -3261,7 +3261,7 @@
         <v>52</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>53</v>
@@ -3317,8 +3317,8 @@
       <c r="AA18" s="5">
         <v>12</v>
       </c>
-      <c r="AB18" s="5" t="s">
-        <v>60</v>
+      <c r="AB18" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC18" s="5">
         <v>12</v>
@@ -3327,16 +3327,16 @@
         <v>0</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG18" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AH18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI18" s="5" t="s">
         <v>53</v>

</xml_diff>